<commit_message>
Resources - Update Planilla
</commit_message>
<xml_diff>
--- a/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
+++ b/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
@@ -1,31 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Autodesk\Revit\Addins\2021\QCReinforcement2.0.0.0\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48706643-89D6-4361-B3E5-E0BF63208C76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-94" yWindow="-94" windowWidth="19380" windowHeight="10380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
     <sheet name="Fehab" sheetId="7" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="QCEMPLEADOS">[1]Datos!$A$1:$A$10</definedName>
-    <definedName name="SIDEREMPLEADOS">[1]Datos!$C$1:$C$6</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>UBICACION</t>
   </si>
@@ -161,9 +153,6 @@
     <t>PESO TOTAL (kg)</t>
   </si>
   <si>
-    <t>FEHAB</t>
-  </si>
-  <si>
     <t>CANT:</t>
   </si>
   <si>
@@ -176,16 +165,16 @@
     <t>_______</t>
   </si>
   <si>
-    <t>____________</t>
-  </si>
-  <si>
     <t>______</t>
+  </si>
+  <si>
+    <t>PLANILLA FEHAB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -554,30 +543,10 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="QC_Tabla" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="QC_Tabla" xfId="2"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color auto="1"/>
@@ -677,14 +646,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
+    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10">
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
-    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
+    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1061,106 +1030,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="QC-Resumen"/>
-      <sheetName val="QC-Planilla"/>
-      <sheetName val="QC-Pegar"/>
-      <sheetName val="RVT"/>
-      <sheetName val="TK"/>
-      <sheetName val="RebarGroup"/>
-      <sheetName val="Datos"/>
-      <sheetName val="QC-Planilla_old"/>
-      <sheetName val="CAD"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Alfonso Jurado</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Ivan Macalupu</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Carlos Gines</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Juan Pozo</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Edson Mamani</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>Omar Alvarado</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Fernando Romero</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>Rafael Palacios</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Franklin Cabrera</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>Susan Minaya</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Hitlier Neyra</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>Victor Otero</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Jorge Sulca</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Moises Vasquez</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Neyser Yupanqui</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Victor Angulo</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Franklin James Cabrera Bravo" refreshedDate="44160.987504050929" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{332BBB87-4D27-4228-B5A6-83E7F3810EE0}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franklin James Cabrera Bravo" refreshedDate="44160.987504050929" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A3:AB9999" sheet="Fehab"/>
   </cacheSource>
@@ -1303,7 +1174,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0AA2CB95-D1C5-4EC0-A0CD-A4345619E9DE}" name="TD_Structure" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TD_Structure" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="I13:L16" firstHeaderRow="2" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="29">
     <pivotField axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1481,10 +1352,10 @@
     <dataField name="PESO TOTAL (kg)" fld="25" baseField="2" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="2">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1501,7 +1372,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5D8AE520-4425-4CE1-B3BD-0E2E53248407}" name="TablaDinámica1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="D13:E16" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="29">
     <pivotField compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1671,10 +1542,10 @@
     <dataField name="PESO TOTAL (kg)" fld="25" baseField="26" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="7">
+    <format dxfId="0">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1952,39 +1823,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q26"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L16" sqref="I16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.61328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.61328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.4609375" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.61328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.6328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.86328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.1328125" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.86328125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.61328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.84375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.3828125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.15234375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.4609375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.84375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.61328125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
     </row>
-    <row r="3" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N3" s="17" t="s">
         <v>24</v>
       </c>
@@ -1993,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N4" s="17" t="s">
         <v>32</v>
       </c>
@@ -2002,15 +1873,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N5" s="17" t="s">
         <v>25</v>
       </c>
       <c r="O5" s="20"/>
     </row>
-    <row r="6" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="7" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.149999999999999" x14ac:dyDescent="0.4">
       <c r="B8" s="42" t="s">
         <v>27</v>
       </c>
@@ -2028,7 +1899,7 @@
       <c r="N8" s="42"/>
       <c r="O8" s="42"/>
     </row>
-    <row r="11" spans="2:17" ht="13.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:17" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="21" t="s">
         <v>28</v>
       </c>
@@ -2045,7 +1916,7 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C12" s="29"/>
       <c r="F12" s="30"/>
       <c r="H12" s="29"/>
@@ -2056,7 +1927,7 @@
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
     </row>
-    <row r="13" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D13" s="24" t="s">
         <v>40</v>
       </c>
@@ -2073,7 +1944,7 @@
       <c r="P13"/>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D14" s="24" t="s">
         <v>20</v>
       </c>
@@ -2098,7 +1969,7 @@
       <c r="P14"/>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
         <v>31</v>
       </c>
@@ -2119,7 +1990,7 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D16" s="35" t="s">
         <v>30</v>
       </c>
@@ -2136,49 +2007,49 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="17" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="18" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="19" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="20" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="21" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="22" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="23" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F23"/>
       <c r="G23"/>
       <c r="I23"/>
@@ -2187,7 +2058,7 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="24" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" s="32"/>
@@ -2201,7 +2072,7 @@
       <c r="P24" s="32"/>
       <c r="Q24" s="32"/>
     </row>
-    <row r="25" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="25" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F25"/>
       <c r="G25"/>
       <c r="I25"/>
@@ -2210,7 +2081,7 @@
       <c r="L25"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="26" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F26"/>
       <c r="G26"/>
     </row>
@@ -2226,44 +2097,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2882A094-2BCC-46A2-BEAB-D78C47F0F159}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6328125" defaultRowHeight="14" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.61328125" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.58984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.2265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.61328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.23046875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.15234375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6328125" style="3" customWidth="1"/>
-    <col min="10" max="18" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.6796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12.36328125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.6328125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="11.6328125" style="3"/>
-    <col min="28" max="28" width="11.6328125" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="11.6328125" style="3"/>
+    <col min="8" max="8" width="7.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.61328125" style="3" customWidth="1"/>
+    <col min="10" max="18" width="4.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.4609375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12.3828125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="11.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.23046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.61328125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="11.61328125" style="3"/>
+    <col min="28" max="28" width="11.61328125" style="3" customWidth="1"/>
+    <col min="29" max="16384" width="11.61328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="60" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:28" ht="59.6" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="12" t="s">
@@ -2275,46 +2146,46 @@
         <v>10</v>
       </c>
       <c r="H1" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="T1" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="S1" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="41" t="s">
-        <v>47</v>
-      </c>
       <c r="U1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="V1" s="38">
         <f>+SUM(W4:W9999)</f>
@@ -2334,7 +2205,7 @@
       <c r="AA1" s="40"/>
       <c r="AB1" s="15"/>
     </row>
-    <row r="2" spans="1:28" ht="14.95" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -2358,11 +2229,8 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
-      <c r="X2" s="3" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="3" spans="1:28" ht="14.95" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Management - Error carpeta TEP
</commit_message>
<xml_diff>
--- a/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
+++ b/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Autodesk\Revit\Addins\2021\QCReinforcement2.0.0.0\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E789788-AE06-496C-A941-71B801FD2AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-94" yWindow="-94" windowWidth="19380" windowHeight="10380" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
-    <sheet name="Fehab" sheetId="7" r:id="rId2"/>
+    <sheet name="QC-Planilla" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -174,12 +175,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +328,20 @@
       <name val="Futura Bk BT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -446,7 +461,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -485,9 +500,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -540,13 +552,42 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="QC_Tabla" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="QC_Tabla" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -646,14 +687,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
+    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
+    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1031,9 +1072,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franklin James Cabrera Bravo" refreshedDate="44160.987504050929" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Franklin James Cabrera Bravo" refreshedDate="44187.003299652781" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:AB9999" sheet="Fehab"/>
+    <worksheetSource ref="A3:AB9999" sheet="QC-Planilla"/>
   </cacheSource>
   <cacheFields count="29">
     <cacheField name="UBICACION" numFmtId="0">
@@ -1174,7 +1215,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TD_Structure" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="TD_Structure" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="I13:L16" firstHeaderRow="2" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="29">
     <pivotField axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1352,10 +1393,10 @@
     <dataField name="PESO TOTAL (kg)" fld="25" baseField="2" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1372,7 +1413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="D13:E16" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="29">
     <pivotField compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -1542,10 +1583,10 @@
     <dataField name="PESO TOTAL (kg)" fld="25" baseField="26" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="0">
+    <format dxfId="7">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1823,116 +1864,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q26"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L16" sqref="I16:L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="6.61328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.58984375" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.61328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.4609375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.58984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.61328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.58984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.61328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.84375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.3828125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.15234375" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.4609375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.84375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15.61328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.58984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.36328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.1328125" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.58984375" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+    <row r="1" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
+    <row r="2" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="N3" s="17" t="s">
+    <row r="3" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+      <c r="N3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="19">
-        <f>Fehab!AA1</f>
+      <c r="O3" s="18">
+        <f>'QC-Planilla'!AA1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="N4" s="17" t="s">
+    <row r="4" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+      <c r="N4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="18">
-        <f>Fehab!E1</f>
+      <c r="O4" s="17">
+        <f>'QC-Planilla'!E1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="N5" s="17" t="s">
+    <row r="5" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+      <c r="N5" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="20"/>
+      <c r="O5" s="19"/>
     </row>
-    <row r="6" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.149999999999999" x14ac:dyDescent="0.4">
-      <c r="B8" s="42" t="s">
+    <row r="6" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
+    <row r="7" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
+    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.5" x14ac:dyDescent="0.75">
+      <c r="B8" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
     </row>
-    <row r="11" spans="2:17" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="21" t="s">
+    <row r="11" spans="2:17" ht="13.75" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="H11" s="21" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="H11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="C12" s="29"/>
-      <c r="F12" s="30"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="C12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
     </row>
-    <row r="13" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="D13" s="24" t="s">
+    <row r="13" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+      <c r="D13" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E13"/>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J13"/>
@@ -1944,20 +1985,20 @@
       <c r="P13"/>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="D14" s="24" t="s">
+    <row r="14" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+      <c r="D14" s="23" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="23" t="s">
         <v>2</v>
       </c>
       <c r="L14" t="s">
@@ -1969,11 +2010,11 @@
       <c r="P14"/>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="25"/>
+      <c r="E15" s="24"/>
       <c r="I15" t="s">
         <v>31</v>
       </c>
@@ -1983,73 +2024,73 @@
       <c r="K15" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="25"/>
+      <c r="L15" s="24"/>
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="D16" s="35" t="s">
+    <row r="16" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+      <c r="D16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="I16" s="35" t="s">
+      <c r="E16" s="35"/>
+      <c r="I16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="36"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="17" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="18" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="19" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="20" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="21" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="22" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="23" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="F23"/>
       <c r="G23"/>
       <c r="I23"/>
@@ -2058,21 +2099,21 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="24" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="F24"/>
       <c r="G24"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
     </row>
-    <row r="25" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="25" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="F25"/>
       <c r="G25"/>
       <c r="I25"/>
@@ -2081,7 +2122,7 @@
       <c r="L25"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
+    <row r="26" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
       <c r="F26"/>
       <c r="G26"/>
     </row>
@@ -2097,40 +2138,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.61328125" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.58984375" defaultRowHeight="14" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="24.61328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.61328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.23046875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.15234375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.58984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.58984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.2265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.6796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.61328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.61328125" style="3" customWidth="1"/>
-    <col min="10" max="18" width="4.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.15234375" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.4609375" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12.3828125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.61328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.23046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.61328125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="11.61328125" style="3"/>
-    <col min="28" max="28" width="11.61328125" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="11.61328125" style="3"/>
+    <col min="8" max="8" width="7.58984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.58984375" style="3" customWidth="1"/>
+    <col min="10" max="18" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6.6796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.453125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12.36328125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="11.58984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.2265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.58984375" style="3" customWidth="1"/>
+    <col min="27" max="27" width="19.1328125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="21.2265625" style="44" customWidth="1"/>
+    <col min="29" max="16384" width="11.58984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="59.6" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:28" ht="60" x14ac:dyDescent="0.6">
+      <c r="A1" s="33" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2142,59 +2183,59 @@
       </c>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="40" t="s">
         <v>45</v>
       </c>
       <c r="U1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="38">
+      <c r="V1" s="37">
         <f>+SUM(W4:W9999)</f>
         <v>0</v>
       </c>
       <c r="W1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="39">
+      <c r="X1" s="38">
         <f>+SUM(Z4:Z9999)/1000</f>
         <v>0</v>
       </c>
@@ -2202,10 +2243,10 @@
       <c r="Z1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="15"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="43"/>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -2230,89 +2271,89 @@
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="N3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="O3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="R3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="28" t="s">
+      <c r="S3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="28" t="s">
+      <c r="T3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="37" t="s">
+      <c r="U3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="V3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="26" t="s">
+      <c r="W3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="27" t="s">
+      <c r="X3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="Y3" s="27" t="s">
+      <c r="Y3" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="28" t="s">
+      <c r="Z3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="AA3" s="28" t="s">
+      <c r="AA3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="28" t="s">
+      <c r="AB3" s="42" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Management - Update Planilla
</commit_message>
<xml_diff>
--- a/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
+++ b/QCReinforcement2.0.0.0/Resources/QC_Planilla.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Autodesk\Revit\Addins\2021\QCReinforcement2.0.0.0\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QC-James\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E789788-AE06-496C-A941-71B801FD2AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-94" yWindow="-94" windowWidth="19380" windowHeight="10380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="3" r:id="rId1"/>
     <sheet name="QC-Planilla" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>UBICACION</t>
   </si>
@@ -49,9 +49,6 @@
     <t>FORMA</t>
   </si>
   <si>
-    <t>R. ESP</t>
-  </si>
-  <si>
     <t>RADIO</t>
   </si>
   <si>
@@ -94,12 +91,6 @@
     <t>PLANO</t>
   </si>
   <si>
-    <t>N°EL</t>
-  </si>
-  <si>
-    <t>PZAxELEM</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>PESO (kg)</t>
-  </si>
-  <si>
     <t>RESUMEN</t>
   </si>
   <si>
@@ -136,12 +124,6 @@
     <t>LONGxPIEZA</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>DIAM.</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -170,12 +152,36 @@
   </si>
   <si>
     <t>PLANILLA FEHAB</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>N°ELEM</t>
+  </si>
+  <si>
+    <t>R.ESP</t>
+  </si>
+  <si>
+    <t>PZAxELE</t>
+  </si>
+  <si>
+    <t>C.TOTAL</t>
+  </si>
+  <si>
+    <t>DIAMETRO</t>
+  </si>
+  <si>
+    <t>PESOT.</t>
+  </si>
+  <si>
+    <t>OP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -549,25 +555,115 @@
     <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="QC_Tabla" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="QC_Tabla" xfId="2"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -687,14 +783,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
+    <tableStyle name="QC_Style_Segmentacion" pivot="0" table="0" count="10">
+      <tableStyleElement type="wholeTable" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
     </tableStyle>
-    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
+    <tableStyle name="QC_Tabla_Dinamica" pivot="0" count="3">
+      <tableStyleElement type="wholeTable" dxfId="28"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="totalRow" dxfId="26"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1024,8 +1120,8 @@
       <xdr:rowOff>158432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1351880</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>799819</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>614045</xdr:rowOff>
     </xdr:to>
@@ -1072,11 +1168,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Franklin James Cabrera Bravo" refreshedDate="44187.003299652781" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="QC-James" refreshedDate="44232.680509490739" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:AB9999" sheet="QC-Planilla"/>
+    <worksheetSource ref="B3:AD9999" sheet="QC-Planilla"/>
   </cacheSource>
-  <cacheFields count="29">
+  <cacheFields count="30">
     <cacheField name="UBICACION" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
         <m/>
@@ -1095,7 +1191,7 @@
     <cacheField name="TIPO" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="N°EL" numFmtId="0">
+    <cacheField name="N°ELEM" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="CODIGO" numFmtId="0">
@@ -1104,7 +1200,7 @@
     <cacheField name="FORMA" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="R. ESP" numFmtId="0">
+    <cacheField name="R.ESP" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="RADIO" numFmtId="0">
@@ -1146,25 +1242,136 @@
     <cacheField name="GAMMA" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="PZAxELEM" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="TOTAL" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="DIAM." numFmtId="0">
+    <cacheField name="PZAxELE" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="C.TOTAL" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="DIAMETRO" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="LONGxPIEZA" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
-    <cacheField name="PESO (kg)" numFmtId="0">
+    <cacheField name="PESOT." numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="PLANO" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
         <m/>
       </sharedItems>
+    </cacheField>
+    <cacheField name="OP" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="ID" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Campo1" numFmtId="0" formula=" 0" databaseField="0"/>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="QC-James" refreshedDate="44232.681642592594" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A3:AD9999" sheet="QC-Planilla"/>
+  </cacheSource>
+  <cacheFields count="31">
+    <cacheField name="ITEM" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="UBICACION" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="NIVEL" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="APLICACIÓN" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="TIPO" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="N°ELEM" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="CODIGO" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="FORMA" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="R.ESP" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="RADIO" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="A" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="B" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="C" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="D" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="E" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="F" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="G" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="H" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="I" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="ALFA" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="BETA" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="GAMMA" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="PZAxELE" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="C.TOTAL" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="DIAMETRO" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LONGxPIEZA" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="PESOT." numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="PLANO" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="OP" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
     <cacheField name="ID" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
@@ -1180,7 +1387,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1209,15 +1416,53 @@
     <m/>
     <m/>
     <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
     <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="TD_Structure" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TD_Structure" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="I13:L16" firstHeaderRow="2" firstDataRow="2" firstDataCol="3"/>
-  <pivotFields count="29">
+  <pivotFields count="30">
     <pivotField axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
@@ -1255,13 +1500,7 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1362,12 +1601,13 @@
         </ext>
       </extLst>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField name="PESO (kg)2" dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
@@ -1393,10 +1633,10 @@
     <dataField name="PESO TOTAL (kg)" fld="25" baseField="2" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="25">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1413,9 +1653,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" grandTotalCaption="Total" updatedVersion="6" minRefreshableVersion="3" showDrill="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" gridDropZones="1">
   <location ref="D13:E16" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="29">
+  <pivotFields count="31">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1444,13 +1685,7 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
-          <x14:pivotField fillDownLabels="1"/>
-        </ext>
-      </extLst>
-    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1551,22 +1786,23 @@
         </ext>
       </extLst>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField name="PESO (kg)2" dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="2">
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="26"/>
+    <field x="27"/>
   </rowFields>
   <rowItems count="2">
     <i>
@@ -1580,13 +1816,13 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="PESO TOTAL (kg)" fld="25" baseField="26" baseItem="0"/>
+    <dataField name="PESO TOTAL (kg)" fld="26" baseField="27" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="7">
+    <format dxfId="20">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -1864,91 +2100,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:Q25"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L16" sqref="I16:L16"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.58984375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="6.61328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.58984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.61328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.4609375" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.58984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="6.61328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.58984375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.1328125" style="2" customWidth="1"/>
-    <col min="12" max="13" width="11.453125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.81640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15.58984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.61328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.84375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.3828125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.15234375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.4609375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.84375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.61328125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N3" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O3" s="18">
-        <f>'QC-Planilla'!AA1</f>
+        <f>'QC-Planilla'!AB1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N4" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O4" s="17">
-        <f>'QC-Planilla'!E1</f>
+        <f>'QC-Planilla'!F1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35">
       <c r="N5" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O5" s="19"/>
     </row>
-    <row r="6" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="7" spans="2:17" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.6"/>
-    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.5" x14ac:dyDescent="0.75">
-      <c r="B8" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
+    <row r="6" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:17" s="1" customFormat="1" ht="14.15" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="2:17" s="4" customFormat="1" ht="20.149999999999999" x14ac:dyDescent="0.4">
+      <c r="B8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
     </row>
-    <row r="11" spans="2:17" ht="13.75" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:17" ht="13.3" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="21"/>
       <c r="H11" s="20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
@@ -1957,7 +2193,7 @@
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="C12" s="28"/>
       <c r="F12" s="29"/>
       <c r="H12" s="28"/>
@@ -1968,13 +2204,16 @@
       <c r="M12" s="29"/>
       <c r="N12" s="29"/>
     </row>
-    <row r="13" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D13" s="23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
       <c r="I13" s="23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J13"/>
       <c r="K13"/>
@@ -1985,13 +2224,16 @@
       <c r="P13"/>
       <c r="Q13"/>
     </row>
-    <row r="14" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D14" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
       <c r="I14" s="23" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2244,7 @@
         <v>2</v>
       </c>
       <c r="L14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
@@ -2010,19 +2252,22 @@
       <c r="P14"/>
       <c r="Q14"/>
     </row>
-    <row r="15" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E15" s="24"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
       <c r="I15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L15" s="24"/>
       <c r="M15"/>
@@ -2031,13 +2276,16 @@
       <c r="P15"/>
       <c r="Q15"/>
     </row>
-    <row r="16" spans="2:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="16" spans="2:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D16" s="34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" s="35"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
       <c r="I16" s="34" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -2048,49 +2296,49 @@
       <c r="P16"/>
       <c r="Q16"/>
     </row>
-    <row r="17" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="17" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="18" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="19" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="20" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="21" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="22" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="23" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F23"/>
       <c r="G23"/>
       <c r="I23"/>
@@ -2099,7 +2347,7 @@
       <c r="L23"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="24" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" s="31"/>
@@ -2113,7 +2361,7 @@
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
     </row>
-    <row r="25" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
+    <row r="25" spans="6:17" ht="14.6" x14ac:dyDescent="0.4">
       <c r="F25"/>
       <c r="G25"/>
       <c r="I25"/>
@@ -2121,10 +2369,6 @@
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
-    </row>
-    <row r="26" spans="6:17" ht="14.75" x14ac:dyDescent="0.75">
-      <c r="F26"/>
-      <c r="G26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2138,121 +2382,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" defaultGridColor="0" colorId="9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.58984375" defaultRowHeight="14" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.61328125" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.58984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.58984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.2265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.6796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.58984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.58984375" style="3" customWidth="1"/>
-    <col min="10" max="18" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.6796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.453125" style="3" customWidth="1"/>
-    <col min="23" max="23" width="12.36328125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="11.58984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.2265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.58984375" style="3" customWidth="1"/>
-    <col min="27" max="27" width="19.1328125" style="3" customWidth="1"/>
-    <col min="28" max="28" width="21.2265625" style="44" customWidth="1"/>
-    <col min="29" max="16384" width="11.58984375" style="3"/>
+    <col min="1" max="1" width="7.765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.61328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.23046875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.15234375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.61328125" style="3" customWidth="1"/>
+    <col min="11" max="19" width="4.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="6.69140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.15234375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.4609375" style="3" customWidth="1"/>
+    <col min="24" max="24" width="12.3828125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="11.61328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.23046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.61328125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="19.15234375" style="3" customWidth="1"/>
+    <col min="29" max="29" width="13.84375" style="3" customWidth="1"/>
+    <col min="30" max="30" width="21.23046875" style="43" customWidth="1"/>
+    <col min="31" max="16384" width="11.61328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="60" x14ac:dyDescent="0.6">
-      <c r="A1" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:30" ht="59.6" x14ac:dyDescent="0.35">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="37">
-        <f>+SUM(W4:W9999)</f>
+      <c r="U1" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="37">
+        <f>+SUM(X4:X9999)</f>
         <v>0</v>
       </c>
-      <c r="W1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="38">
-        <f>+SUM(Z4:Z9999)/1000</f>
+      <c r="X1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="38">
+        <f>+SUM(AA4:AA9999)/1000</f>
         <v>0</v>
       </c>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="43"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="42"/>
     </row>
-    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2264,97 +2512,104 @@
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="9"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="H3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="I3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="K3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="L3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="M3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="N3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="O3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="P3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="Q3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="R3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="S3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="T3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="27" t="s">
+      <c r="U3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="V3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="W3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z3" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA3" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB3" s="42" t="s">
-        <v>37</v>
+      <c r="AC3" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD3" s="41" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>